<commit_message>
Documentation and other minor updates
</commit_message>
<xml_diff>
--- a/sprites and sounds.xlsx
+++ b/sprites and sounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spwil\Documents\Tangerine\Projects - Boulder Dash\OricBoulderDash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEB8951-077C-409E-AF5B-ECFEA2D51F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965A6970-36D0-4C93-9AE6-A8A79F350CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" activeTab="5" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
   </bookViews>
   <sheets>
     <sheet name="Oric BD tiles plan" sheetId="5" r:id="rId1"/>
@@ -1380,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5927D687-0E20-461F-BF7C-9EB33D57AC1C}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -55228,7 +55228,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADF9F42-C143-4CDD-8ACB-7652330B2E87}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -55257,22 +55259,22 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
-        <v>3000</v>
+        <v>2300</v>
       </c>
       <c r="B2" s="24">
         <v>448</v>
       </c>
       <c r="C2">
         <f>HEX2DEC(A2)</f>
-        <v>12288</v>
+        <v>8960</v>
       </c>
       <c r="D2" t="str">
         <f>DEC2HEX(C2,4)</f>
-        <v>3000</v>
+        <v>2300</v>
       </c>
       <c r="E2" t="str">
         <f>"$"&amp;LOWER(LEFT(D2,2))</f>
-        <v>$30</v>
+        <v>$23</v>
       </c>
       <c r="F2" t="str">
         <f>"$"&amp;LOWER(MID(D2,3,2))</f>
@@ -55285,15 +55287,15 @@
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C3">
         <f>C2+$B$2</f>
-        <v>12736</v>
+        <v>9408</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D22" si="0">DEC2HEX(C3,4)</f>
-        <v>31C0</v>
+        <v>24C0</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E22" si="1">"$"&amp;LOWER(LEFT(D3,2))</f>
-        <v>$31</v>
+        <v>$24</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F22" si="2">"$"&amp;LOWER(MID(D3,3,2))</f>
@@ -55301,90 +55303,90 @@
       </c>
       <c r="H3" s="25" t="str" cm="1">
         <f t="array" ref="H3:AE3">CONCATENATE(TRANSPOSE(E2:E25),", ")</f>
-        <v xml:space="preserve">$30, </v>
+        <v xml:space="preserve">$23, </v>
       </c>
       <c r="I3" s="25" t="str">
+        <v xml:space="preserve">$24, </v>
+      </c>
+      <c r="J3" s="25" t="str">
+        <v xml:space="preserve">$26, </v>
+      </c>
+      <c r="K3" s="25" t="str">
+        <v xml:space="preserve">$28, </v>
+      </c>
+      <c r="L3" s="25" t="str">
+        <v xml:space="preserve">$2a, </v>
+      </c>
+      <c r="M3" s="25" t="str">
+        <v xml:space="preserve">$2b, </v>
+      </c>
+      <c r="N3" s="25" t="str">
+        <v xml:space="preserve">$2d, </v>
+      </c>
+      <c r="O3" s="25" t="str">
+        <v xml:space="preserve">$2f, </v>
+      </c>
+      <c r="P3" s="25" t="str">
         <v xml:space="preserve">$31, </v>
       </c>
-      <c r="J3" s="25" t="str">
-        <v xml:space="preserve">$33, </v>
-      </c>
-      <c r="K3" s="25" t="str">
-        <v xml:space="preserve">$35, </v>
-      </c>
-      <c r="L3" s="25" t="str">
-        <v xml:space="preserve">$37, </v>
-      </c>
-      <c r="M3" s="25" t="str">
+      <c r="Q3" s="25" t="str">
+        <v xml:space="preserve">$32, </v>
+      </c>
+      <c r="R3" s="25" t="str">
+        <v xml:space="preserve">$34, </v>
+      </c>
+      <c r="S3" s="25" t="str">
+        <v xml:space="preserve">$36, </v>
+      </c>
+      <c r="T3" t="str">
         <v xml:space="preserve">$38, </v>
       </c>
-      <c r="N3" s="25" t="str">
-        <v xml:space="preserve">$3a, </v>
-      </c>
-      <c r="O3" s="25" t="str">
-        <v xml:space="preserve">$3c, </v>
-      </c>
-      <c r="P3" s="25" t="str">
-        <v xml:space="preserve">$3e, </v>
-      </c>
-      <c r="Q3" s="25" t="str">
+      <c r="U3" t="str">
+        <v xml:space="preserve">$39, </v>
+      </c>
+      <c r="V3" t="str">
+        <v xml:space="preserve">$3b, </v>
+      </c>
+      <c r="W3" t="str">
+        <v xml:space="preserve">$3d, </v>
+      </c>
+      <c r="X3" t="str">
         <v xml:space="preserve">$3f, </v>
       </c>
-      <c r="R3" s="25" t="str">
-        <v xml:space="preserve">$41, </v>
-      </c>
-      <c r="S3" s="25" t="str">
-        <v xml:space="preserve">$43, </v>
-      </c>
-      <c r="T3" t="str">
-        <v xml:space="preserve">$45, </v>
-      </c>
-      <c r="U3" t="str">
+      <c r="Y3" t="str">
+        <v xml:space="preserve">$40, </v>
+      </c>
+      <c r="Z3" t="str">
+        <v xml:space="preserve">$42, </v>
+      </c>
+      <c r="AA3" t="str">
+        <v xml:space="preserve">$44, </v>
+      </c>
+      <c r="AB3" t="str">
         <v xml:space="preserve">$46, </v>
       </c>
-      <c r="V3" t="str">
-        <v xml:space="preserve">$48, </v>
-      </c>
-      <c r="W3" t="str">
-        <v xml:space="preserve">$4a, </v>
-      </c>
-      <c r="X3" t="str">
-        <v xml:space="preserve">$4c, </v>
-      </c>
-      <c r="Y3" t="str">
-        <v xml:space="preserve">$4d, </v>
-      </c>
-      <c r="Z3" t="str">
-        <v xml:space="preserve">$4f, </v>
-      </c>
-      <c r="AA3" t="str">
-        <v xml:space="preserve">$51, </v>
-      </c>
-      <c r="AB3" t="str">
-        <v xml:space="preserve">$53, </v>
-      </c>
       <c r="AC3" t="str">
-        <v xml:space="preserve">$54, </v>
+        <v xml:space="preserve">$47, </v>
       </c>
       <c r="AD3" t="str">
-        <v xml:space="preserve">$56, </v>
+        <v xml:space="preserve">$49, </v>
       </c>
       <c r="AE3" t="str">
-        <v xml:space="preserve">$58, </v>
+        <v xml:space="preserve">$4b, </v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C4">
         <f t="shared" ref="C4:C25" si="3">C3+$B$2</f>
-        <v>13184</v>
+        <v>9856</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>3380</v>
+        <v>2680</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>$33</v>
+        <v>$26</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -55394,15 +55396,15 @@
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C5">
         <f t="shared" si="3"/>
-        <v>13632</v>
+        <v>10304</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>3540</v>
+        <v>2840</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>$35</v>
+        <v>$28</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -55415,15 +55417,15 @@
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C6">
         <f t="shared" si="3"/>
-        <v>14080</v>
+        <v>10752</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>3700</v>
+        <v>2A00</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>$37</v>
+        <v>$2a</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -55506,15 +55508,15 @@
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C7">
         <f t="shared" si="3"/>
-        <v>14528</v>
+        <v>11200</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>38C0</v>
+        <v>2BC0</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>$38</v>
+        <v>$2b</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -55524,15 +55526,15 @@
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" si="3"/>
-        <v>14976</v>
+        <v>11648</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>3A80</v>
+        <v>2D80</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>$3a</v>
+        <v>$2d</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -55542,15 +55544,15 @@
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="3"/>
-        <v>15424</v>
+        <v>12096</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>3C40</v>
+        <v>2F40</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>$3c</v>
+        <v>$2f</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -55560,15 +55562,15 @@
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="3"/>
-        <v>15872</v>
+        <v>12544</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>3E00</v>
+        <v>3100</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>$3e</v>
+        <v>$31</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -55578,15 +55580,15 @@
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="3"/>
-        <v>16320</v>
+        <v>12992</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>3FC0</v>
+        <v>32C0</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>$3f</v>
+        <v>$32</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -55596,15 +55598,15 @@
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C12">
         <f t="shared" si="3"/>
-        <v>16768</v>
+        <v>13440</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>4180</v>
+        <v>3480</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>$41</v>
+        <v>$34</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -55614,15 +55616,15 @@
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" si="3"/>
-        <v>17216</v>
+        <v>13888</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>4340</v>
+        <v>3640</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>$43</v>
+        <v>$36</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -55632,15 +55634,15 @@
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C14">
         <f t="shared" si="3"/>
-        <v>17664</v>
+        <v>14336</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>3800</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>$45</v>
+        <v>$38</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -55650,15 +55652,15 @@
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C15">
         <f t="shared" si="3"/>
-        <v>18112</v>
+        <v>14784</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>46C0</v>
+        <v>39C0</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>$46</v>
+        <v>$39</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -55668,15 +55670,15 @@
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C16">
         <f t="shared" si="3"/>
-        <v>18560</v>
+        <v>15232</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>4880</v>
+        <v>3B80</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>$48</v>
+        <v>$3b</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -55686,15 +55688,15 @@
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C17">
         <f t="shared" si="3"/>
-        <v>19008</v>
+        <v>15680</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>4A40</v>
+        <v>3D40</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>$4a</v>
+        <v>$3d</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -55704,15 +55706,15 @@
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C18">
         <f t="shared" si="3"/>
-        <v>19456</v>
+        <v>16128</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>4C00</v>
+        <v>3F00</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>$4c</v>
+        <v>$3f</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -55722,15 +55724,15 @@
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="3"/>
-        <v>19904</v>
+        <v>16576</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>4DC0</v>
+        <v>40C0</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>$4d</v>
+        <v>$40</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
@@ -55740,15 +55742,15 @@
     <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C20">
         <f t="shared" si="3"/>
-        <v>20352</v>
+        <v>17024</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>4F80</v>
+        <v>4280</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>$4f</v>
+        <v>$42</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
@@ -55758,15 +55760,15 @@
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C21">
         <f t="shared" si="3"/>
-        <v>20800</v>
+        <v>17472</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>5140</v>
+        <v>4440</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>$51</v>
+        <v>$44</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
@@ -55776,15 +55778,15 @@
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C22">
         <f t="shared" si="3"/>
-        <v>21248</v>
+        <v>17920</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>5300</v>
+        <v>4600</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>$53</v>
+        <v>$46</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
@@ -55794,15 +55796,15 @@
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C23">
         <f t="shared" si="3"/>
-        <v>21696</v>
+        <v>18368</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ref="D23:D25" si="4">DEC2HEX(C23,4)</f>
-        <v>54C0</v>
+        <v>47C0</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" ref="E23:E25" si="5">"$"&amp;LOWER(LEFT(D23,2))</f>
-        <v>$54</v>
+        <v>$47</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" ref="F23:F25" si="6">"$"&amp;LOWER(MID(D23,3,2))</f>
@@ -55812,15 +55814,15 @@
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C24">
         <f t="shared" si="3"/>
-        <v>22144</v>
+        <v>18816</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="4"/>
-        <v>5680</v>
+        <v>4980</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>$56</v>
+        <v>$49</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="6"/>
@@ -55830,15 +55832,15 @@
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C25">
         <f t="shared" si="3"/>
-        <v>22592</v>
+        <v>19264</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="4"/>
-        <v>5840</v>
+        <v>4B40</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>$58</v>
+        <v>$4b</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Instructions added, Oric 1 fixes applies
</commit_message>
<xml_diff>
--- a/sprites and sounds.xlsx
+++ b/sprites and sounds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spwil\Documents\Tangerine\Projects - Boulder Dash\OricBoulderDash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E6E06-A38D-4777-A7CC-23E301268189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45030EA0-1F24-4E9D-8E48-FD2AF09EA03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" activeTab="5" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
   </bookViews>
   <sheets>
     <sheet name="Oric BD tiles plan" sheetId="5" r:id="rId1"/>
@@ -1397,11 +1397,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5927D687-0E20-461F-BF7C-9EB33D57AC1C}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57644,9 +57644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADF9F42-C143-4CDD-8ACB-7652330B2E87}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -57675,22 +57673,22 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
-        <v>2700</v>
+        <v>3900</v>
       </c>
       <c r="B2" s="24">
         <v>448</v>
       </c>
       <c r="C2">
         <f>HEX2DEC(A2)</f>
-        <v>9984</v>
+        <v>14592</v>
       </c>
       <c r="D2" t="str">
         <f>DEC2HEX(C2,4)</f>
-        <v>2700</v>
+        <v>3900</v>
       </c>
       <c r="E2" t="str">
         <f>"$"&amp;LOWER(LEFT(D2,2))</f>
-        <v>$27</v>
+        <v>$39</v>
       </c>
       <c r="F2" t="str">
         <f>"$"&amp;LOWER(MID(D2,3,2))</f>
@@ -57703,15 +57701,15 @@
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C3">
         <f>C2+$B$2</f>
-        <v>10432</v>
+        <v>15040</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D22" si="0">DEC2HEX(C3,4)</f>
-        <v>28C0</v>
+        <v>3AC0</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E22" si="1">"$"&amp;LOWER(LEFT(D3,2))</f>
-        <v>$28</v>
+        <v>$3a</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F22" si="2">"$"&amp;LOWER(MID(D3,3,2))</f>
@@ -57719,90 +57717,90 @@
       </c>
       <c r="H3" s="25" t="str" cm="1">
         <f t="array" ref="H3:AE3">CONCATENATE(TRANSPOSE(E2:E25),", ")</f>
-        <v xml:space="preserve">$27, </v>
+        <v xml:space="preserve">$39, </v>
       </c>
       <c r="I3" s="25" t="str">
-        <v xml:space="preserve">$28, </v>
+        <v xml:space="preserve">$3a, </v>
       </c>
       <c r="J3" s="25" t="str">
-        <v xml:space="preserve">$2a, </v>
+        <v xml:space="preserve">$3c, </v>
       </c>
       <c r="K3" s="25" t="str">
-        <v xml:space="preserve">$2c, </v>
+        <v xml:space="preserve">$3e, </v>
       </c>
       <c r="L3" s="25" t="str">
-        <v xml:space="preserve">$2e, </v>
+        <v xml:space="preserve">$40, </v>
       </c>
       <c r="M3" s="25" t="str">
-        <v xml:space="preserve">$2f, </v>
+        <v xml:space="preserve">$41, </v>
       </c>
       <c r="N3" s="25" t="str">
-        <v xml:space="preserve">$31, </v>
+        <v xml:space="preserve">$43, </v>
       </c>
       <c r="O3" s="25" t="str">
-        <v xml:space="preserve">$33, </v>
+        <v xml:space="preserve">$45, </v>
       </c>
       <c r="P3" s="25" t="str">
-        <v xml:space="preserve">$35, </v>
+        <v xml:space="preserve">$47, </v>
       </c>
       <c r="Q3" s="25" t="str">
-        <v xml:space="preserve">$36, </v>
+        <v xml:space="preserve">$48, </v>
       </c>
       <c r="R3" s="25" t="str">
-        <v xml:space="preserve">$38, </v>
+        <v xml:space="preserve">$4a, </v>
       </c>
       <c r="S3" s="25" t="str">
-        <v xml:space="preserve">$3a, </v>
+        <v xml:space="preserve">$4c, </v>
       </c>
       <c r="T3" t="str">
-        <v xml:space="preserve">$3c, </v>
+        <v xml:space="preserve">$4e, </v>
       </c>
       <c r="U3" t="str">
-        <v xml:space="preserve">$3d, </v>
+        <v xml:space="preserve">$4f, </v>
       </c>
       <c r="V3" t="str">
-        <v xml:space="preserve">$3f, </v>
+        <v xml:space="preserve">$51, </v>
       </c>
       <c r="W3" t="str">
-        <v xml:space="preserve">$41, </v>
+        <v xml:space="preserve">$53, </v>
       </c>
       <c r="X3" t="str">
-        <v xml:space="preserve">$43, </v>
+        <v xml:space="preserve">$55, </v>
       </c>
       <c r="Y3" t="str">
-        <v xml:space="preserve">$44, </v>
+        <v xml:space="preserve">$56, </v>
       </c>
       <c r="Z3" t="str">
-        <v xml:space="preserve">$46, </v>
+        <v xml:space="preserve">$58, </v>
       </c>
       <c r="AA3" t="str">
-        <v xml:space="preserve">$48, </v>
+        <v xml:space="preserve">$5a, </v>
       </c>
       <c r="AB3" t="str">
-        <v xml:space="preserve">$4a, </v>
+        <v xml:space="preserve">$5c, </v>
       </c>
       <c r="AC3" t="str">
-        <v xml:space="preserve">$4b, </v>
+        <v xml:space="preserve">$5d, </v>
       </c>
       <c r="AD3" t="str">
-        <v xml:space="preserve">$4d, </v>
+        <v xml:space="preserve">$5f, </v>
       </c>
       <c r="AE3" t="str">
-        <v xml:space="preserve">$4f, </v>
+        <v xml:space="preserve">$61, </v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C4">
         <f t="shared" ref="C4:C25" si="3">C3+$B$2</f>
-        <v>10880</v>
+        <v>15488</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>2A80</v>
+        <v>3C80</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>$2a</v>
+        <v>$3c</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -57812,15 +57810,15 @@
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C5">
         <f t="shared" si="3"/>
-        <v>11328</v>
+        <v>15936</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>2C40</v>
+        <v>3E40</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>$2c</v>
+        <v>$3e</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -57833,15 +57831,15 @@
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C6">
         <f t="shared" si="3"/>
-        <v>11776</v>
+        <v>16384</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>2E00</v>
+        <v>4000</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>$2e</v>
+        <v>$40</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -57924,15 +57922,15 @@
     <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C7">
         <f t="shared" si="3"/>
-        <v>12224</v>
+        <v>16832</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>2FC0</v>
+        <v>41C0</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>$2f</v>
+        <v>$41</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -57942,15 +57940,15 @@
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" si="3"/>
-        <v>12672</v>
+        <v>17280</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>3180</v>
+        <v>4380</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>$31</v>
+        <v>$43</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -57960,15 +57958,15 @@
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="3"/>
-        <v>13120</v>
+        <v>17728</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>3340</v>
+        <v>4540</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>$33</v>
+        <v>$45</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -57978,15 +57976,15 @@
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="3"/>
-        <v>13568</v>
+        <v>18176</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>3500</v>
+        <v>4700</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>$35</v>
+        <v>$47</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -57996,15 +57994,15 @@
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="3"/>
-        <v>14016</v>
+        <v>18624</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>36C0</v>
+        <v>48C0</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>$36</v>
+        <v>$48</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -58014,15 +58012,15 @@
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C12">
         <f t="shared" si="3"/>
-        <v>14464</v>
+        <v>19072</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>3880</v>
+        <v>4A80</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>$38</v>
+        <v>$4a</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -58032,15 +58030,15 @@
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" si="3"/>
-        <v>14912</v>
+        <v>19520</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>3A40</v>
+        <v>4C40</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>$3a</v>
+        <v>$4c</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -58050,15 +58048,15 @@
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C14">
         <f t="shared" si="3"/>
-        <v>15360</v>
+        <v>19968</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>3C00</v>
+        <v>4E00</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>$3c</v>
+        <v>$4e</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -58068,15 +58066,15 @@
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C15">
         <f t="shared" si="3"/>
-        <v>15808</v>
+        <v>20416</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>3DC0</v>
+        <v>4FC0</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>$3d</v>
+        <v>$4f</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -58086,15 +58084,15 @@
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C16">
         <f t="shared" si="3"/>
-        <v>16256</v>
+        <v>20864</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>3F80</v>
+        <v>5180</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>$3f</v>
+        <v>$51</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -58104,15 +58102,15 @@
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C17">
         <f t="shared" si="3"/>
-        <v>16704</v>
+        <v>21312</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>4140</v>
+        <v>5340</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>$41</v>
+        <v>$53</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -58122,15 +58120,15 @@
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C18">
         <f t="shared" si="3"/>
-        <v>17152</v>
+        <v>21760</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>4300</v>
+        <v>5500</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>$43</v>
+        <v>$55</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -58140,15 +58138,15 @@
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="3"/>
-        <v>17600</v>
+        <v>22208</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>44C0</v>
+        <v>56C0</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>$44</v>
+        <v>$56</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
@@ -58158,15 +58156,15 @@
     <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C20">
         <f t="shared" si="3"/>
-        <v>18048</v>
+        <v>22656</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>4680</v>
+        <v>5880</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>$46</v>
+        <v>$58</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
@@ -58176,15 +58174,15 @@
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C21">
         <f t="shared" si="3"/>
-        <v>18496</v>
+        <v>23104</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>4840</v>
+        <v>5A40</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>$48</v>
+        <v>$5a</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
@@ -58194,15 +58192,15 @@
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C22">
         <f t="shared" si="3"/>
-        <v>18944</v>
+        <v>23552</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>4A00</v>
+        <v>5C00</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>$4a</v>
+        <v>$5c</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
@@ -58212,15 +58210,15 @@
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C23">
         <f t="shared" si="3"/>
-        <v>19392</v>
+        <v>24000</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" ref="D23:D25" si="4">DEC2HEX(C23,4)</f>
-        <v>4BC0</v>
+        <v>5DC0</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" ref="E23:E25" si="5">"$"&amp;LOWER(LEFT(D23,2))</f>
-        <v>$4b</v>
+        <v>$5d</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" ref="F23:F25" si="6">"$"&amp;LOWER(MID(D23,3,2))</f>
@@ -58230,15 +58228,15 @@
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C24">
         <f t="shared" si="3"/>
-        <v>19840</v>
+        <v>24448</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="4"/>
-        <v>4D80</v>
+        <v>5F80</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="5"/>
-        <v>$4d</v>
+        <v>$5f</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="6"/>
@@ -58248,15 +58246,15 @@
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C25">
         <f t="shared" si="3"/>
-        <v>20288</v>
+        <v>24896</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="4"/>
-        <v>4F40</v>
+        <v>6140</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="5"/>
-        <v>$4f</v>
+        <v>$61</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Title screen theme music added
</commit_message>
<xml_diff>
--- a/sprites and sounds.xlsx
+++ b/sprites and sounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spwil\Documents\Tangerine\Projects - Boulder Dash\OricBoulderDash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45030EA0-1F24-4E9D-8E48-FD2AF09EA03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A65E164-05DC-4802-830D-9CE98B5A64EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" activeTab="5" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="790" activeTab="4" xr2:uid="{9987D57F-F998-4D92-8F32-7F5C1DED2F39}"/>
   </bookViews>
   <sheets>
     <sheet name="Oric BD tiles plan" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="252">
   <si>
     <t>Dirt</t>
   </si>
@@ -353,9 +353,6 @@
     <t>Actor</t>
   </si>
   <si>
-    <t>Sound attributes</t>
-  </si>
-  <si>
     <t>Sound event</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
   </si>
   <si>
     <t>CB</t>
-  </si>
-  <si>
-    <t>* Also see sfxgen.tap to use settings and play back</t>
   </si>
   <si>
     <t>CBA</t>
@@ -775,6 +769,62 @@
   <si>
     <t>100000</t>
   </si>
+  <si>
+    <t>Sound attributes using SFXGEN.TAP utility</t>
+  </si>
+  <si>
+    <t>0 to 31</t>
+  </si>
+  <si>
+    <t>0 to 15, 
+16 = use envelope</t>
+  </si>
+  <si>
+    <t>8 to 15</t>
+  </si>
+  <si>
+    <t>Value depends on selected combination</t>
+  </si>
+  <si>
+    <t>A = $7e</t>
+  </si>
+  <si>
+    <t>B = $7d</t>
+  </si>
+  <si>
+    <t>C = $7b</t>
+  </si>
+  <si>
+    <t>AB = $7c</t>
+  </si>
+  <si>
+    <t>pitch a</t>
+  </si>
+  <si>
+    <t>pitch b</t>
+  </si>
+  <si>
+    <t>normal AB = $7c</t>
+  </si>
+  <si>
+    <t>2 bytes 
+(low, high)</t>
+  </si>
+  <si>
+    <t>Byte sequence from SFXGEN and in program</t>
+  </si>
+  <si>
+    <t>0 and 1</t>
+  </si>
+  <si>
+    <t>2 and 3</t>
+  </si>
+  <si>
+    <t>4 and 5</t>
+  </si>
+  <si>
+    <t>11 and 12</t>
+  </si>
 </sst>
 </file>
 
@@ -795,7 +845,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,8 +888,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -941,11 +997,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1024,6 +1104,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1513,7 +1612,7 @@
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1527,7 +1626,7 @@
         <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1541,7 +1640,7 @@
         <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4698,7 +4797,7 @@
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q38" s="6"/>
       <c r="AF38" t="str">
@@ -5242,7 +5341,7 @@
         <v>2B</v>
       </c>
       <c r="AF44" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.3">
@@ -50311,7 +50410,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" t="str">
         <f>";"&amp;A1</f>
@@ -50320,14 +50419,14 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B9" si="0">LOWER(BIN2HEX(A2,2))</f>
         <v>00</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" ref="D2:K2">CONCATENATE("$",TRANSPOSE(B2:B9),", ")</f>
@@ -50357,7 +50456,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
@@ -50366,7 +50465,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -50375,7 +50474,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -50384,7 +50483,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -50393,7 +50492,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -50402,7 +50501,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -50411,7 +50510,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -50420,7 +50519,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C11" t="str">
         <f>";"&amp;A11</f>
@@ -50429,14 +50528,14 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B12" t="str">
         <f>LOWER(BIN2HEX(A12,2))</f>
         <v>0c</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" ref="D12:K12">CONCATENATE("$",TRANSPOSE(B12:B19),", ")</f>
@@ -50466,7 +50565,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" ref="B13:B19" si="1">LOWER(BIN2HEX(A13,2))</f>
@@ -50475,7 +50574,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="1"/>
@@ -50484,7 +50583,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
@@ -50493,7 +50592,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
@@ -50502,7 +50601,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
@@ -50511,7 +50610,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="1"/>
@@ -50520,7 +50619,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="1"/>
@@ -50532,7 +50631,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C21" t="str">
         <f>";"&amp;A21</f>
@@ -50541,14 +50640,14 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B22" t="str">
         <f>LOWER(BIN2HEX(A22,2))</f>
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" ref="D22:K22">CONCATENATE("$",TRANSPOSE(B22:B29),", ")</f>
@@ -50578,7 +50677,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" ref="B23:B29" si="2">LOWER(BIN2HEX(A23,2))</f>
@@ -50587,7 +50686,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="2"/>
@@ -50596,7 +50695,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="2"/>
@@ -50605,7 +50704,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="2"/>
@@ -50614,7 +50713,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="2"/>
@@ -50623,7 +50722,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="2"/>
@@ -50632,7 +50731,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="2"/>
@@ -50644,7 +50743,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C31" t="str">
         <f>";"&amp;A31</f>
@@ -50653,14 +50752,14 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B32" t="str">
         <f>LOWER(BIN2HEX(A32,2))</f>
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" ref="D32:K32">CONCATENATE("$",TRANSPOSE(B32:B39),", ")</f>
@@ -50690,7 +50789,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" ref="B33:B39" si="3">LOWER(BIN2HEX(A33,2))</f>
@@ -50699,7 +50798,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="3"/>
@@ -50708,7 +50807,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="3"/>
@@ -50717,7 +50816,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="3"/>
@@ -50726,7 +50825,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="3"/>
@@ -50735,7 +50834,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="3"/>
@@ -50744,7 +50843,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="3"/>
@@ -50756,7 +50855,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C41" t="str">
         <f>";"&amp;A41</f>
@@ -50765,14 +50864,14 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B42" t="str">
         <f>LOWER(BIN2HEX(A42,2))</f>
         <v>08</v>
       </c>
       <c r="C42" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D42" t="str" cm="1">
         <f t="array" ref="D42:K42">CONCATENATE("$",TRANSPOSE(B42:B49),", ")</f>
@@ -50802,7 +50901,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" ref="B43:B49" si="4">LOWER(BIN2HEX(A43,2))</f>
@@ -50811,7 +50910,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="4"/>
@@ -50820,7 +50919,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="4"/>
@@ -50829,7 +50928,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="4"/>
@@ -50838,7 +50937,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="4"/>
@@ -50847,7 +50946,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="4"/>
@@ -50856,7 +50955,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="4"/>
@@ -50868,7 +50967,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C51" t="str">
         <f>";"&amp;A51</f>
@@ -50877,14 +50976,14 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B52" t="str">
         <f>LOWER(BIN2HEX(A52,2))</f>
         <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D52" t="str" cm="1">
         <f t="array" ref="D52:K52">CONCATENATE("$",TRANSPOSE(B52:B59),", ")</f>
@@ -50914,7 +51013,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" ref="B53:B59" si="5">LOWER(BIN2HEX(A53,2))</f>
@@ -50923,7 +51022,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="5"/>
@@ -50932,7 +51031,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="5"/>
@@ -50941,7 +51040,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="5"/>
@@ -50950,7 +51049,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="5"/>
@@ -50959,7 +51058,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="5"/>
@@ -50968,7 +51067,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="5"/>
@@ -50980,7 +51079,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C61" t="str">
         <f>";"&amp;A61</f>
@@ -50989,14 +51088,14 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B62" t="str">
         <f>LOWER(BIN2HEX(A62,2))</f>
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D62" t="str" cm="1">
         <f t="array" ref="D62:K62">CONCATENATE("$",TRANSPOSE(B62:B69),", ")</f>
@@ -51026,7 +51125,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" ref="B63:B69" si="6">LOWER(BIN2HEX(A63,2))</f>
@@ -51035,7 +51134,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="6"/>
@@ -51044,7 +51143,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="6"/>
@@ -51053,7 +51152,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="6"/>
@@ -51062,7 +51161,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="6"/>
@@ -51071,7 +51170,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="6"/>
@@ -51080,7 +51179,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="6"/>
@@ -51092,7 +51191,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C71" t="str">
         <f>";"&amp;A71</f>
@@ -51101,14 +51200,14 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B72" t="str">
         <f>LOWER(BIN2HEX(A72,2))</f>
         <v>0c</v>
       </c>
       <c r="C72" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D72" t="str" cm="1">
         <f t="array" ref="D72:K72">CONCATENATE("$",TRANSPOSE(B72:B79),", ")</f>
@@ -51138,7 +51237,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" ref="B73:B79" si="7">LOWER(BIN2HEX(A73,2))</f>
@@ -51147,7 +51246,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="7"/>
@@ -51156,7 +51255,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="7"/>
@@ -51165,7 +51264,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="7"/>
@@ -51174,7 +51273,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="7"/>
@@ -51183,7 +51282,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="7"/>
@@ -51192,7 +51291,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="7"/>
@@ -51204,7 +51303,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C81" t="str">
         <f>";"&amp;A81</f>
@@ -51213,14 +51312,14 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B82" t="str">
         <f>LOWER(BIN2HEX(A82,2))</f>
         <v>08</v>
       </c>
       <c r="C82" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D82" t="str" cm="1">
         <f t="array" ref="D82:K82">CONCATENATE("$",TRANSPOSE(B82:B89),", ")</f>
@@ -51250,7 +51349,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" ref="B83:B89" si="8">LOWER(BIN2HEX(A83,2))</f>
@@ -51259,7 +51358,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="8"/>
@@ -51268,7 +51367,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="8"/>
@@ -51277,7 +51376,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="8"/>
@@ -51286,7 +51385,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="8"/>
@@ -51295,7 +51394,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="8"/>
@@ -51304,7 +51403,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="8"/>
@@ -51316,7 +51415,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C91" t="str">
         <f>";"&amp;A91</f>
@@ -51325,14 +51424,14 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B92" t="str">
         <f>LOWER(BIN2HEX(A92,2))</f>
         <v>08</v>
       </c>
       <c r="C92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D92" t="str" cm="1">
         <f t="array" ref="D92:K92">CONCATENATE("$",TRANSPOSE(B92:B99),", ")</f>
@@ -51362,7 +51461,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" ref="B93:B99" si="9">LOWER(BIN2HEX(A93,2))</f>
@@ -51371,7 +51470,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="9"/>
@@ -51380,7 +51479,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="9"/>
@@ -51389,7 +51488,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="9"/>
@@ -51398,7 +51497,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" si="9"/>
@@ -51407,7 +51506,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="9"/>
@@ -51416,7 +51515,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="9"/>
@@ -51428,7 +51527,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C101" t="str">
         <f>";"&amp;A101</f>
@@ -51437,14 +51536,14 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B102" t="str">
         <f>LOWER(BIN2HEX(A102,2))</f>
         <v>08</v>
       </c>
       <c r="C102" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D102" t="str" cm="1">
         <f t="array" ref="D102:K102">CONCATENATE("$",TRANSPOSE(B102:B109),", ")</f>
@@ -51474,7 +51573,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" ref="B103:B109" si="10">LOWER(BIN2HEX(A103,2))</f>
@@ -51483,7 +51582,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="10"/>
@@ -51492,7 +51591,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="10"/>
@@ -51501,7 +51600,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="10"/>
@@ -51510,7 +51609,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="10"/>
@@ -51519,7 +51618,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="10"/>
@@ -51528,7 +51627,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="10"/>
@@ -51540,7 +51639,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C111" t="str">
         <f>";"&amp;A111</f>
@@ -51549,14 +51648,14 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B112" t="str">
         <f>LOWER(BIN2HEX(A112,2))</f>
         <v>00</v>
       </c>
       <c r="C112" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D112" t="str" cm="1">
         <f t="array" ref="D112:K112">CONCATENATE("$",TRANSPOSE(B112:B119),", ")</f>
@@ -51586,7 +51685,7 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" ref="B113:B119" si="11">LOWER(BIN2HEX(A113,2))</f>
@@ -51595,7 +51694,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="11"/>
@@ -51604,7 +51703,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B115" t="str">
         <f t="shared" si="11"/>
@@ -51613,7 +51712,7 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B116" t="str">
         <f t="shared" si="11"/>
@@ -51622,7 +51721,7 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B117" t="str">
         <f t="shared" si="11"/>
@@ -51631,7 +51730,7 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="11"/>
@@ -51640,7 +51739,7 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="11"/>
@@ -51652,7 +51751,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C121" t="str">
         <f>";"&amp;A121</f>
@@ -51662,14 +51761,14 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B122" t="str">
         <f>LOWER(BIN2HEX(A122,2))</f>
         <v>00</v>
       </c>
       <c r="C122" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D122" t="str" cm="1">
         <f t="array" ref="D122:K122">CONCATENATE("$",TRANSPOSE(B122:B129),", ")</f>
@@ -51699,7 +51798,7 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B123" t="str">
         <f t="shared" ref="B123:B129" si="12">LOWER(BIN2HEX(A123,2))</f>
@@ -51708,7 +51807,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B124" t="str">
         <f t="shared" si="12"/>
@@ -51717,7 +51816,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B125" t="str">
         <f t="shared" si="12"/>
@@ -51726,7 +51825,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B126" t="str">
         <f t="shared" si="12"/>
@@ -51735,7 +51834,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B127" t="str">
         <f t="shared" si="12"/>
@@ -51744,7 +51843,7 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="12"/>
@@ -51753,7 +51852,7 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="12"/>
@@ -51762,7 +51861,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C131" t="str">
         <f>";"&amp;A131</f>
@@ -51771,14 +51870,14 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B132" t="str">
         <f>LOWER(BIN2HEX(A132,2))</f>
         <v>00</v>
       </c>
       <c r="C132" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D132" t="str" cm="1">
         <f t="array" ref="D132:K132">CONCATENATE("$",TRANSPOSE(B132:B139),", ")</f>
@@ -51808,7 +51907,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B133" t="str">
         <f t="shared" ref="B133:B139" si="13">LOWER(BIN2HEX(A133,2))</f>
@@ -51817,7 +51916,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B134" t="str">
         <f t="shared" si="13"/>
@@ -51826,7 +51925,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B135" t="str">
         <f t="shared" si="13"/>
@@ -51835,7 +51934,7 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B136" t="str">
         <f t="shared" si="13"/>
@@ -51844,7 +51943,7 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B137" t="str">
         <f t="shared" si="13"/>
@@ -51853,7 +51952,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B138" t="str">
         <f t="shared" si="13"/>
@@ -51862,7 +51961,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B139" t="str">
         <f t="shared" si="13"/>
@@ -51871,7 +51970,7 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C141" t="str">
         <f>";"&amp;A141</f>
@@ -51880,14 +51979,14 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B142" t="str">
         <f>LOWER(BIN2HEX(A142,2))</f>
         <v>00</v>
       </c>
       <c r="C142" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D142" t="str" cm="1">
         <f t="array" ref="D142:K142">CONCATENATE("$",TRANSPOSE(B142:B149),", ")</f>
@@ -51917,7 +52016,7 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B143" t="str">
         <f t="shared" ref="B143:B149" si="14">LOWER(BIN2HEX(A143,2))</f>
@@ -51926,7 +52025,7 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B144" t="str">
         <f t="shared" si="14"/>
@@ -51935,7 +52034,7 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B145" t="str">
         <f t="shared" si="14"/>
@@ -51944,7 +52043,7 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B146" t="str">
         <f t="shared" si="14"/>
@@ -51953,7 +52052,7 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B147" t="str">
         <f t="shared" si="14"/>
@@ -51962,7 +52061,7 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B148" t="str">
         <f t="shared" si="14"/>
@@ -51971,7 +52070,7 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B149" t="str">
         <f t="shared" si="14"/>
@@ -51980,7 +52079,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C151" t="str">
         <f>";"&amp;A151</f>
@@ -51989,14 +52088,14 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B152" t="str">
         <f>LOWER(BIN2HEX(A152,2))</f>
         <v>00</v>
       </c>
       <c r="C152" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D152" t="str" cm="1">
         <f t="array" ref="D152:K152">CONCATENATE("$",TRANSPOSE(B152:B159),", ")</f>
@@ -52026,7 +52125,7 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B153" t="str">
         <f t="shared" ref="B153:B159" si="15">LOWER(BIN2HEX(A153,2))</f>
@@ -52035,7 +52134,7 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B154" t="str">
         <f t="shared" si="15"/>
@@ -52044,7 +52143,7 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B155" t="str">
         <f t="shared" si="15"/>
@@ -52053,7 +52152,7 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B156" t="str">
         <f t="shared" si="15"/>
@@ -52062,7 +52161,7 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B157" t="str">
         <f t="shared" si="15"/>
@@ -52071,7 +52170,7 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B158" t="str">
         <f t="shared" si="15"/>
@@ -52080,7 +52179,7 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B159" t="str">
         <f t="shared" si="15"/>
@@ -52101,14 +52200,14 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B162" t="str">
         <f>LOWER(BIN2HEX(A162,2))</f>
         <v>1c</v>
       </c>
       <c r="C162" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D162" t="str" cm="1">
         <f t="array" ref="D162:K162">CONCATENATE("$",TRANSPOSE(B162:B169),", ")</f>
@@ -52183,7 +52282,7 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B168" t="str">
         <f t="shared" si="16"/>
@@ -52192,7 +52291,7 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B169" t="str">
         <f t="shared" si="16"/>
@@ -52210,14 +52309,14 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B172" t="str">
         <f>LOWER(BIN2HEX(A172,2))</f>
         <v>08</v>
       </c>
       <c r="C172" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D172" t="str" cm="1">
         <f t="array" ref="D172:K172">CONCATENATE("$",TRANSPOSE(B172:B179),", ")</f>
@@ -52247,7 +52346,7 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B173" t="str">
         <f t="shared" ref="B173:B179" si="17">LOWER(BIN2HEX(A173,2))</f>
@@ -52256,7 +52355,7 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="17"/>
@@ -52265,7 +52364,7 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="17"/>
@@ -52274,7 +52373,7 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="17"/>
@@ -52301,7 +52400,7 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="17"/>
@@ -52329,7 +52428,7 @@
         <v>3c</v>
       </c>
       <c r="C182" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D182" t="str" cm="1">
         <f t="array" ref="D182:K182">CONCATENATE("$",TRANSPOSE(B182:B189),", ")</f>
@@ -52368,7 +52467,7 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="18"/>
@@ -52377,7 +52476,7 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="18"/>
@@ -52413,7 +52512,7 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="18"/>
@@ -52438,7 +52537,7 @@
         <v>3e</v>
       </c>
       <c r="C192" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D192" t="str" cm="1">
         <f t="array" ref="D192:K192">CONCATENATE("$",TRANSPOSE(B192:B199),", ")</f>
@@ -52468,7 +52567,7 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B193" t="str">
         <f t="shared" ref="B193:B199" si="19">LOWER(BIN2HEX(A193,2))</f>
@@ -52477,7 +52576,7 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B194" t="str">
         <f t="shared" si="19"/>
@@ -52486,7 +52585,7 @@
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B195" t="str">
         <f t="shared" si="19"/>
@@ -52522,7 +52621,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B199" t="str">
         <f t="shared" si="19"/>
@@ -52547,7 +52646,7 @@
         <v>20</v>
       </c>
       <c r="C202" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D202" t="str" cm="1">
         <f t="array" ref="D202:K202">CONCATENATE("$",TRANSPOSE(B202:B209),", ")</f>
@@ -52604,7 +52703,7 @@
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B206" t="str">
         <f t="shared" si="20"/>
@@ -52613,7 +52712,7 @@
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B207" t="str">
         <f t="shared" si="20"/>
@@ -52622,7 +52721,7 @@
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B208" t="str">
         <f t="shared" si="20"/>
@@ -52631,7 +52730,7 @@
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B209" t="str">
         <f t="shared" si="20"/>
@@ -52656,7 +52755,7 @@
         <v>3e</v>
       </c>
       <c r="C212" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D212" t="str" cm="1">
         <f t="array" ref="D212:K212">CONCATENATE("$",TRANSPOSE(B212:B219),", ")</f>
@@ -52704,7 +52803,7 @@
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B215" t="str">
         <f t="shared" si="21"/>
@@ -52740,7 +52839,7 @@
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A219" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B219" t="str">
         <f t="shared" si="21"/>
@@ -52758,14 +52857,14 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A222" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B222" t="str">
         <f>LOWER(BIN2HEX(A222,2))</f>
         <v>1c</v>
       </c>
       <c r="C222" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D222" t="str" cm="1">
         <f t="array" ref="D222:K222">CONCATENATE("$",TRANSPOSE(B222:B229),", ")</f>
@@ -52849,7 +52948,7 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B229" t="str">
         <f t="shared" si="22"/>
@@ -52874,7 +52973,7 @@
         <v>3e</v>
       </c>
       <c r="C232" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D232" t="str" cm="1">
         <f t="array" ref="D232:K232">CONCATENATE("$",TRANSPOSE(B232:B239),", ")</f>
@@ -52904,7 +53003,7 @@
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A233" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B233" t="str">
         <f t="shared" ref="B233:B239" si="23">LOWER(BIN2HEX(A233,2))</f>
@@ -52913,7 +53012,7 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A234" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B234" t="str">
         <f t="shared" si="23"/>
@@ -52922,7 +53021,7 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B235" t="str">
         <f t="shared" si="23"/>
@@ -52958,7 +53057,7 @@
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B239" t="str">
         <f t="shared" si="23"/>
@@ -52976,14 +53075,14 @@
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B242" t="str">
         <f>LOWER(BIN2HEX(A242,2))</f>
         <v>1c</v>
       </c>
       <c r="C242" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D242" t="str" cm="1">
         <f t="array" ref="D242:K242">CONCATENATE("$",TRANSPOSE(B242:B249),", ")</f>
@@ -53022,7 +53121,7 @@
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B244" t="str">
         <f t="shared" si="24"/>
@@ -53058,7 +53157,7 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B248" t="str">
         <f t="shared" si="24"/>
@@ -53067,7 +53166,7 @@
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B249" t="str">
         <f t="shared" si="24"/>
@@ -53085,14 +53184,14 @@
     </row>
     <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B252" t="str">
         <f>LOWER(BIN2HEX(A252,2))</f>
         <v>1c</v>
       </c>
       <c r="C252" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D252" t="str" cm="1">
         <f t="array" ref="D252:K252">CONCATENATE("$",TRANSPOSE(B252:B259),", ")</f>
@@ -53149,7 +53248,7 @@
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B256" t="str">
         <f t="shared" si="25"/>
@@ -53158,7 +53257,7 @@
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B257" t="str">
         <f t="shared" si="25"/>
@@ -53176,7 +53275,7 @@
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B259" t="str">
         <f t="shared" si="25"/>
@@ -53185,7 +53284,7 @@
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C261" t="str">
         <f>";"&amp;A261</f>
@@ -53194,14 +53293,14 @@
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A262" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B262" t="str">
         <f>LOWER(BIN2HEX(A262,2))</f>
         <v>00</v>
       </c>
       <c r="C262" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D262" t="str" cm="1">
         <f t="array" ref="D262:K262">CONCATENATE("$",TRANSPOSE(B262:B269),", ")</f>
@@ -53231,7 +53330,7 @@
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B263" t="str">
         <f t="shared" ref="B263:B269" si="26">LOWER(BIN2HEX(A263,2))</f>
@@ -53240,7 +53339,7 @@
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B264" t="str">
         <f t="shared" si="26"/>
@@ -53249,7 +53348,7 @@
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B265" t="str">
         <f t="shared" si="26"/>
@@ -53258,7 +53357,7 @@
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B266" t="str">
         <f t="shared" si="26"/>
@@ -53267,7 +53366,7 @@
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B267" t="str">
         <f t="shared" si="26"/>
@@ -53276,7 +53375,7 @@
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B268" t="str">
         <f t="shared" si="26"/>
@@ -53285,7 +53384,7 @@
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B269" t="str">
         <f t="shared" si="26"/>
@@ -53294,7 +53393,7 @@
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C271" t="str">
         <f>";"&amp;A271</f>
@@ -53303,14 +53402,14 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B272" t="str">
         <f>LOWER(BIN2HEX(A272,2))</f>
         <v>00</v>
       </c>
       <c r="C272" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D272" t="str" cm="1">
         <f t="array" ref="D272:K272">CONCATENATE("$",TRANSPOSE(B272:B279),", ")</f>
@@ -53340,7 +53439,7 @@
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B273" t="str">
         <f t="shared" ref="B273:B279" si="27">LOWER(BIN2HEX(A273,2))</f>
@@ -53349,7 +53448,7 @@
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B274" t="str">
         <f t="shared" si="27"/>
@@ -53358,7 +53457,7 @@
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B275" t="str">
         <f t="shared" si="27"/>
@@ -53367,7 +53466,7 @@
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B276" t="str">
         <f t="shared" si="27"/>
@@ -53376,7 +53475,7 @@
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B277" t="str">
         <f t="shared" si="27"/>
@@ -53385,7 +53484,7 @@
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B278" t="str">
         <f t="shared" si="27"/>
@@ -53394,7 +53493,7 @@
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B279" t="str">
         <f t="shared" si="27"/>
@@ -53403,7 +53502,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" s="28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C281" t="str">
         <f>";"&amp;A281</f>
@@ -53412,14 +53511,14 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B282" t="str">
         <f>LOWER(BIN2HEX(A282,2))</f>
         <v>06</v>
       </c>
       <c r="C282" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D282" t="str" cm="1">
         <f t="array" ref="D282:K282">CONCATENATE("$",TRANSPOSE(B282:B289),", ")</f>
@@ -53449,7 +53548,7 @@
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B283" t="str">
         <f t="shared" ref="B283:B289" si="28">LOWER(BIN2HEX(A283,2))</f>
@@ -53458,7 +53557,7 @@
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B284" t="str">
         <f t="shared" si="28"/>
@@ -53476,7 +53575,7 @@
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B286" t="str">
         <f t="shared" si="28"/>
@@ -53485,7 +53584,7 @@
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B287" t="str">
         <f t="shared" si="28"/>
@@ -53494,7 +53593,7 @@
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B288" t="str">
         <f t="shared" si="28"/>
@@ -53503,7 +53602,7 @@
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B289" t="str">
         <f t="shared" si="28"/>
@@ -53512,7 +53611,7 @@
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C291" t="str">
         <f>";"&amp;A291</f>
@@ -53521,14 +53620,14 @@
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B292" t="str">
         <f>LOWER(BIN2HEX(A292,2))</f>
         <v>00</v>
       </c>
       <c r="C292" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D292" t="str" cm="1">
         <f t="array" ref="D292:K292">CONCATENATE("$",TRANSPOSE(B292:B299),", ")</f>
@@ -53558,7 +53657,7 @@
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B293" t="str">
         <f t="shared" ref="B293:B299" si="29">LOWER(BIN2HEX(A293,2))</f>
@@ -53567,7 +53666,7 @@
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B294" t="str">
         <f t="shared" si="29"/>
@@ -53576,7 +53675,7 @@
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B295" t="str">
         <f t="shared" si="29"/>
@@ -53585,7 +53684,7 @@
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A296" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B296" t="str">
         <f t="shared" si="29"/>
@@ -53594,7 +53693,7 @@
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B297" t="str">
         <f t="shared" si="29"/>
@@ -53603,7 +53702,7 @@
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B298" t="str">
         <f t="shared" si="29"/>
@@ -53612,7 +53711,7 @@
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B299" t="str">
         <f t="shared" si="29"/>
@@ -53621,7 +53720,7 @@
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C301" t="str">
         <f>";"&amp;A301</f>
@@ -53637,7 +53736,7 @@
         <v>30</v>
       </c>
       <c r="C302" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D302" t="str" cm="1">
         <f t="array" ref="D302:K302">CONCATENATE("$",TRANSPOSE(B302:B309),", ")</f>
@@ -53667,7 +53766,7 @@
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A303" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B303" t="str">
         <f t="shared" ref="B303:B309" si="30">LOWER(BIN2HEX(A303,2))</f>
@@ -53676,7 +53775,7 @@
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A304" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B304" t="str">
         <f t="shared" si="30"/>
@@ -53685,7 +53784,7 @@
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B305" t="str">
         <f t="shared" si="30"/>
@@ -53694,7 +53793,7 @@
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B306" t="str">
         <f t="shared" si="30"/>
@@ -53703,7 +53802,7 @@
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B307" t="str">
         <f t="shared" si="30"/>
@@ -53721,7 +53820,7 @@
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A309" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B309" t="str">
         <f t="shared" si="30"/>
@@ -53730,7 +53829,7 @@
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C311" t="str">
         <f>";"&amp;A311</f>
@@ -53746,7 +53845,7 @@
         <v>3c</v>
       </c>
       <c r="C312" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D312" t="str" cm="1">
         <f t="array" ref="D312:K312">CONCATENATE("$",TRANSPOSE(B312:B319),", ")</f>
@@ -53776,7 +53875,7 @@
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A313" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B313" t="str">
         <f t="shared" ref="B313:B319" si="31">LOWER(BIN2HEX(A313,2))</f>
@@ -53785,7 +53884,7 @@
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B314" t="str">
         <f t="shared" si="31"/>
@@ -53794,7 +53893,7 @@
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B315" t="str">
         <f t="shared" si="31"/>
@@ -53803,7 +53902,7 @@
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A316" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B316" t="str">
         <f t="shared" si="31"/>
@@ -53812,7 +53911,7 @@
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B317" t="str">
         <f t="shared" si="31"/>
@@ -53821,7 +53920,7 @@
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B318" t="str">
         <f t="shared" si="31"/>
@@ -53830,7 +53929,7 @@
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B319" t="str">
         <f t="shared" si="31"/>
@@ -53839,7 +53938,7 @@
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C321" t="str">
         <f>";"&amp;A321</f>
@@ -53848,14 +53947,14 @@
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B322" t="str">
         <f>LOWER(BIN2HEX(A322,2))</f>
         <v>1c</v>
       </c>
       <c r="C322" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D322" t="str" cm="1">
         <f t="array" ref="D322:K322">CONCATENATE("$",TRANSPOSE(B322:B329),", ")</f>
@@ -53930,7 +54029,7 @@
     </row>
     <row r="328" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A328" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B328" t="str">
         <f t="shared" si="32"/>
@@ -53939,7 +54038,7 @@
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A329" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B329" t="str">
         <f t="shared" si="32"/>
@@ -53948,7 +54047,7 @@
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A331" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C331" t="str">
         <f>";"&amp;A331</f>
@@ -53957,14 +54056,14 @@
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B332" t="str">
         <f>LOWER(BIN2HEX(A332,2))</f>
         <v>1c</v>
       </c>
       <c r="C332" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D332" t="str" cm="1">
         <f t="array" ref="D332:K332">CONCATENATE("$",TRANSPOSE(B332:B339),", ")</f>
@@ -54048,7 +54147,7 @@
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B339" t="str">
         <f t="shared" si="33"/>
@@ -54057,7 +54156,7 @@
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C341" t="str">
         <f>";"&amp;A341</f>
@@ -54073,7 +54172,7 @@
         <v>3c</v>
       </c>
       <c r="C342" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D342" t="str" cm="1">
         <f t="array" ref="D342:K342">CONCATENATE("$",TRANSPOSE(B342:B349),", ")</f>
@@ -54157,7 +54256,7 @@
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B349" t="str">
         <f t="shared" si="34"/>
@@ -54166,7 +54265,7 @@
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C351" t="str">
         <f>";"&amp;A351</f>
@@ -54175,14 +54274,14 @@
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B352" t="str">
         <f>LOWER(BIN2HEX(A352,2))</f>
         <v>1c</v>
       </c>
       <c r="C352" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D352" t="str" cm="1">
         <f t="array" ref="D352:K352">CONCATENATE("$",TRANSPOSE(B352:B359),", ")</f>
@@ -54257,7 +54356,7 @@
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A358" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B358" t="str">
         <f t="shared" si="35"/>
@@ -54266,7 +54365,7 @@
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B359" t="str">
         <f t="shared" si="35"/>
@@ -54275,7 +54374,7 @@
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C361" t="str">
         <f>";"&amp;A361</f>
@@ -54291,7 +54390,7 @@
         <v>38</v>
       </c>
       <c r="C362" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D362" t="str" cm="1">
         <f t="array" ref="D362:K362">CONCATENATE("$",TRANSPOSE(B362:B369),", ")</f>
@@ -54375,7 +54474,7 @@
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B369" t="str">
         <f t="shared" si="36"/>
@@ -54384,7 +54483,7 @@
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A371" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C371" t="str">
         <f>";"&amp;A371</f>
@@ -54400,7 +54499,7 @@
         <v>3e</v>
       </c>
       <c r="C372" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D372" t="str" cm="1">
         <f t="array" ref="D372:K372">CONCATENATE("$",TRANSPOSE(B372:B379),", ")</f>
@@ -54484,7 +54583,7 @@
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A379" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B379" t="str">
         <f t="shared" si="37"/>
@@ -54493,7 +54592,7 @@
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A381" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C381" t="str">
         <f>";"&amp;A381</f>
@@ -54509,7 +54608,7 @@
         <v>3e</v>
       </c>
       <c r="C382" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D382" t="str" cm="1">
         <f t="array" ref="D382:K382">CONCATENATE("$",TRANSPOSE(B382:B389),", ")</f>
@@ -54593,7 +54692,7 @@
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A389" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B389" t="str">
         <f t="shared" si="38"/>
@@ -54602,7 +54701,7 @@
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A391" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C391" t="str">
         <f>";"&amp;A391</f>
@@ -54611,14 +54710,14 @@
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A392" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B392" t="str">
         <f>LOWER(BIN2HEX(A392,2))</f>
         <v>1e</v>
       </c>
       <c r="C392" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D392" t="str" cm="1">
         <f t="array" ref="D392:K392">CONCATENATE("$",TRANSPOSE(B392:B399),", ")</f>
@@ -54693,7 +54792,7 @@
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A398" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B398" t="str">
         <f t="shared" si="39"/>
@@ -54702,7 +54801,7 @@
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A399" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B399" t="str">
         <f t="shared" si="39"/>
@@ -54711,7 +54810,7 @@
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A401" s="28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C401" t="str">
         <f>";"&amp;A401</f>
@@ -54727,7 +54826,7 @@
         <v>36</v>
       </c>
       <c r="C402" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D402" t="str" cm="1">
         <f t="array" ref="D402:K402">CONCATENATE("$",TRANSPOSE(B402:B409),", ")</f>
@@ -54811,7 +54910,7 @@
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A409" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B409" t="str">
         <f t="shared" si="40"/>
@@ -54820,7 +54919,7 @@
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A411" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C411" t="str">
         <f>";"&amp;A411</f>
@@ -54836,7 +54935,7 @@
         <v>3e</v>
       </c>
       <c r="C412" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D412" t="str" cm="1">
         <f t="array" ref="D412:K412">CONCATENATE("$",TRANSPOSE(B412:B419),", ")</f>
@@ -54866,7 +54965,7 @@
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A413" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B413" t="str">
         <f t="shared" ref="B413:B419" si="41">LOWER(BIN2HEX(A413,2))</f>
@@ -54875,7 +54974,7 @@
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A414" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B414" t="str">
         <f t="shared" si="41"/>
@@ -54884,7 +54983,7 @@
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A415" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B415" t="str">
         <f t="shared" si="41"/>
@@ -54893,7 +54992,7 @@
     </row>
     <row r="416" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A416" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B416" t="str">
         <f t="shared" si="41"/>
@@ -54902,7 +55001,7 @@
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A417" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B417" t="str">
         <f t="shared" si="41"/>
@@ -54920,7 +55019,7 @@
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A419" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B419" t="str">
         <f t="shared" si="41"/>
@@ -54929,7 +55028,7 @@
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A421" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C421" t="str">
         <f>";"&amp;A421</f>
@@ -54938,14 +55037,14 @@
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A422" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B422" t="str">
         <f>LOWER(BIN2HEX(A422,2))</f>
         <v>06</v>
       </c>
       <c r="C422" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D422" t="str" cm="1">
         <f t="array" ref="D422:K422">CONCATENATE("$",TRANSPOSE(B422:B429),", ")</f>
@@ -54975,7 +55074,7 @@
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A423" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B423" t="str">
         <f t="shared" ref="B423:B429" si="42">LOWER(BIN2HEX(A423,2))</f>
@@ -54984,7 +55083,7 @@
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A424" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B424" t="str">
         <f t="shared" si="42"/>
@@ -54993,7 +55092,7 @@
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A425" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B425" t="str">
         <f t="shared" si="42"/>
@@ -55020,7 +55119,7 @@
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A428" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B428" t="str">
         <f t="shared" si="42"/>
@@ -55029,7 +55128,7 @@
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A429" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B429" t="str">
         <f t="shared" si="42"/>
@@ -55038,7 +55137,7 @@
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A431" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C431" t="str">
         <f>";"&amp;A431</f>
@@ -55054,7 +55153,7 @@
         <v>36</v>
       </c>
       <c r="C432" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D432" t="str" cm="1">
         <f t="array" ref="D432:K432">CONCATENATE("$",TRANSPOSE(B432:B439),", ")</f>
@@ -55138,7 +55237,7 @@
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A439" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B439" t="str">
         <f t="shared" si="43"/>
@@ -55147,7 +55246,7 @@
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A441" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C441" t="str">
         <f>";"&amp;A441</f>
@@ -55163,7 +55262,7 @@
         <v>30</v>
       </c>
       <c r="C442" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D442" t="str" cm="1">
         <f t="array" ref="D442:K442">CONCATENATE("$",TRANSPOSE(B442:B449),", ")</f>
@@ -55247,7 +55346,7 @@
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A449" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B449" t="str">
         <f t="shared" si="44"/>
@@ -55256,7 +55355,7 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A451" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C451" t="str">
         <f>";"&amp;A451</f>
@@ -55272,7 +55371,7 @@
         <v>22</v>
       </c>
       <c r="C452" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D452" t="str" cm="1">
         <f t="array" ref="D452:K452">CONCATENATE("$",TRANSPOSE(B452:B459),", ")</f>
@@ -55356,7 +55455,7 @@
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A459" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B459" t="str">
         <f t="shared" si="45"/>
@@ -55365,7 +55464,7 @@
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A461" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C461" t="str">
         <f>";"&amp;A461</f>
@@ -55381,7 +55480,7 @@
         <v>26</v>
       </c>
       <c r="C462" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D462" t="str" cm="1">
         <f t="array" ref="D462:K462">CONCATENATE("$",TRANSPOSE(B462:B469),", ")</f>
@@ -55465,7 +55564,7 @@
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A469" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B469" t="str">
         <f t="shared" si="46"/>
@@ -55474,7 +55573,7 @@
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A471" s="28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C471" t="str">
         <f>";"&amp;A471</f>
@@ -55483,14 +55582,14 @@
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A472" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B472" t="str">
         <f>LOWER(BIN2HEX(A472,2))</f>
         <v>1c</v>
       </c>
       <c r="C472" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D472" t="str" cm="1">
         <f t="array" ref="D472:K472">CONCATENATE("$",TRANSPOSE(B472:B479),", ")</f>
@@ -55565,7 +55664,7 @@
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A478" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B478" t="str">
         <f t="shared" si="47"/>
@@ -55574,7 +55673,7 @@
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A479" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B479" t="str">
         <f t="shared" si="47"/>
@@ -55583,7 +55682,7 @@
     </row>
     <row r="481" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A481" s="28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C481" t="str">
         <f>";"&amp;A481</f>
@@ -55599,7 +55698,7 @@
         <v>3c</v>
       </c>
       <c r="C482" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D482" t="str" cm="1">
         <f t="array" ref="D482:K482">CONCATENATE("$",TRANSPOSE(B482:B489),", ")</f>
@@ -55683,7 +55782,7 @@
     </row>
     <row r="489" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A489" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B489" t="str">
         <f t="shared" si="48"/>
@@ -55692,7 +55791,7 @@
     </row>
     <row r="491" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A491" s="28" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C491" t="str">
         <f>";"&amp;A491</f>
@@ -55701,14 +55800,14 @@
     </row>
     <row r="492" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A492" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B492" t="str">
         <f>LOWER(BIN2HEX(A492,2))</f>
         <v>1c</v>
       </c>
       <c r="C492" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D492" t="str" cm="1">
         <f t="array" ref="D492:K492">CONCATENATE("$",TRANSPOSE(B492:B499),", ")</f>
@@ -55783,7 +55882,7 @@
     </row>
     <row r="498" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A498" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B498" t="str">
         <f t="shared" si="49"/>
@@ -55792,7 +55891,7 @@
     </row>
     <row r="499" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A499" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B499" t="str">
         <f t="shared" si="49"/>
@@ -55801,7 +55900,7 @@
     </row>
     <row r="501" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A501" s="28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C501" t="str">
         <f>";"&amp;A501</f>
@@ -55817,7 +55916,7 @@
         <v>3c</v>
       </c>
       <c r="C502" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D502" t="str" cm="1">
         <f t="array" ref="D502:K502">CONCATENATE("$",TRANSPOSE(B502:B509),", ")</f>
@@ -55901,7 +56000,7 @@
     </row>
     <row r="509" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A509" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B509" t="str">
         <f t="shared" si="50"/>
@@ -55910,7 +56009,7 @@
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A511" s="28" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C511" t="str">
         <f>";"&amp;A511</f>
@@ -55919,14 +56018,14 @@
     </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A512" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B512" t="str">
         <f>LOWER(BIN2HEX(A512,2))</f>
         <v>1c</v>
       </c>
       <c r="C512" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D512" t="str" cm="1">
         <f t="array" ref="D512:K512">CONCATENATE("$",TRANSPOSE(B512:B519),", ")</f>
@@ -55965,7 +56064,7 @@
     </row>
     <row r="514" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A514" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B514" t="str">
         <f t="shared" si="51"/>
@@ -55974,7 +56073,7 @@
     </row>
     <row r="515" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A515" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B515" t="str">
         <f t="shared" si="51"/>
@@ -55983,7 +56082,7 @@
     </row>
     <row r="516" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A516" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B516" t="str">
         <f t="shared" si="51"/>
@@ -56010,7 +56109,7 @@
     </row>
     <row r="519" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A519" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B519" t="str">
         <f t="shared" si="51"/>
@@ -56019,7 +56118,7 @@
     </row>
     <row r="521" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A521" s="28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C521" t="str">
         <f>";"&amp;A521</f>
@@ -56035,7 +56134,7 @@
         <v>3e</v>
       </c>
       <c r="C522" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D522" t="str" cm="1">
         <f t="array" ref="D522:K522">CONCATENATE("$",TRANSPOSE(B522:B529),", ")</f>
@@ -56065,7 +56164,7 @@
     </row>
     <row r="523" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A523" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B523" t="str">
         <f t="shared" ref="B523:B529" si="52">LOWER(BIN2HEX(A523,2))</f>
@@ -56074,7 +56173,7 @@
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A524" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B524" t="str">
         <f t="shared" si="52"/>
@@ -56083,7 +56182,7 @@
     </row>
     <row r="525" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A525" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B525" t="str">
         <f t="shared" si="52"/>
@@ -56092,7 +56191,7 @@
     </row>
     <row r="526" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A526" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B526" t="str">
         <f t="shared" si="52"/>
@@ -56101,7 +56200,7 @@
     </row>
     <row r="527" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A527" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B527" t="str">
         <f t="shared" si="52"/>
@@ -56110,7 +56209,7 @@
     </row>
     <row r="528" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A528" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B528" t="str">
         <f t="shared" si="52"/>
@@ -56119,7 +56218,7 @@
     </row>
     <row r="529" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A529" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B529" t="str">
         <f t="shared" si="52"/>
@@ -56128,7 +56227,7 @@
     </row>
     <row r="531" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A531" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C531" t="str">
         <f>";"&amp;A531</f>
@@ -56144,7 +56243,7 @@
         <v>36</v>
       </c>
       <c r="C532" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D532" t="str" cm="1">
         <f t="array" ref="D532:K532">CONCATENATE("$",TRANSPOSE(B532:B539),", ")</f>
@@ -56219,7 +56318,7 @@
     </row>
     <row r="538" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A538" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B538" t="str">
         <f t="shared" si="53"/>
@@ -56228,7 +56327,7 @@
     </row>
     <row r="539" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A539" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B539" t="str">
         <f t="shared" si="53"/>
@@ -56237,7 +56336,7 @@
     </row>
     <row r="541" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A541" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C541" t="str">
         <f>";"&amp;A541</f>
@@ -56253,7 +56352,7 @@
         <v>36</v>
       </c>
       <c r="C542" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D542" t="str" cm="1">
         <f t="array" ref="D542:K542">CONCATENATE("$",TRANSPOSE(B542:B549),", ")</f>
@@ -56319,7 +56418,7 @@
     </row>
     <row r="547" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A547" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B547" t="str">
         <f t="shared" si="54"/>
@@ -56328,7 +56427,7 @@
     </row>
     <row r="548" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A548" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B548" t="str">
         <f t="shared" si="54"/>
@@ -56337,7 +56436,7 @@
     </row>
     <row r="549" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A549" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B549" t="str">
         <f t="shared" si="54"/>
@@ -56346,7 +56445,7 @@
     </row>
     <row r="551" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A551" s="28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C551" t="str">
         <f>";"&amp;A551</f>
@@ -56362,7 +56461,7 @@
         <v>36</v>
       </c>
       <c r="C552" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D552" t="str" cm="1">
         <f t="array" ref="D552:K552">CONCATENATE("$",TRANSPOSE(B552:B559),", ")</f>
@@ -56446,7 +56545,7 @@
     </row>
     <row r="559" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A559" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B559" t="str">
         <f t="shared" si="55"/>
@@ -56455,7 +56554,7 @@
     </row>
     <row r="561" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A561" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C561" t="str">
         <f>";"&amp;A561</f>
@@ -56471,7 +56570,7 @@
         <v>36</v>
       </c>
       <c r="C562" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D562" t="str" cm="1">
         <f t="array" ref="D562:K562">CONCATENATE("$",TRANSPOSE(B562:B569),", ")</f>
@@ -56510,7 +56609,7 @@
     </row>
     <row r="564" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A564" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B564" t="str">
         <f t="shared" si="56"/>
@@ -56519,7 +56618,7 @@
     </row>
     <row r="565" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A565" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B565" t="str">
         <f t="shared" si="56"/>
@@ -56555,7 +56654,7 @@
     </row>
     <row r="569" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A569" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B569" t="str">
         <f t="shared" si="56"/>
@@ -56564,7 +56663,7 @@
     </row>
     <row r="571" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A571" s="28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C571" t="str">
         <f>";"&amp;A571</f>
@@ -56580,7 +56679,7 @@
         <v>36</v>
       </c>
       <c r="C572" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D572" t="str" cm="1">
         <f t="array" ref="D572:K572">CONCATENATE("$",TRANSPOSE(B572:B579),", ")</f>
@@ -56619,7 +56718,7 @@
     </row>
     <row r="574" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A574" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B574" t="str">
         <f t="shared" si="57"/>
@@ -56628,7 +56727,7 @@
     </row>
     <row r="575" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A575" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B575" t="str">
         <f t="shared" si="57"/>
@@ -56664,7 +56763,7 @@
     </row>
     <row r="579" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A579" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B579" t="str">
         <f t="shared" si="57"/>
@@ -56673,7 +56772,7 @@
     </row>
     <row r="581" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A581" s="28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C581" t="str">
         <f>";"&amp;A581</f>
@@ -56689,7 +56788,7 @@
         <v>3e</v>
       </c>
       <c r="C582" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D582" t="str" cm="1">
         <f t="array" ref="D582:K582">CONCATENATE("$",TRANSPOSE(B582:B589),", ")</f>
@@ -56719,7 +56818,7 @@
     </row>
     <row r="583" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A583" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B583" t="str">
         <f t="shared" ref="B583:B589" si="58">LOWER(BIN2HEX(A583,2))</f>
@@ -56728,7 +56827,7 @@
     </row>
     <row r="584" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A584" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B584" t="str">
         <f t="shared" si="58"/>
@@ -56773,7 +56872,7 @@
     </row>
     <row r="589" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A589" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B589" t="str">
         <f t="shared" si="58"/>
@@ -56804,10 +56903,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C1" s="3">
         <v>1024</v>
@@ -56816,15 +56915,15 @@
         <v>128</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="26">
         <v>896</v>
@@ -56833,12 +56932,12 @@
         <v>112</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <f>HEX2DEC(A5)</f>
@@ -56852,12 +56951,12 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B15" si="0">HEX2DEC(A6)</f>
@@ -56871,15 +56970,15 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -56893,15 +56992,15 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -56915,12 +57014,12 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -56934,7 +57033,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -56948,12 +57047,12 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -56967,12 +57066,12 @@
         <v>32</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -56986,12 +57085,12 @@
         <v>32</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -57007,7 +57106,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -57021,12 +57120,12 @@
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -57040,9 +57139,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF4C740-AFD3-4CD2-A94F-EBDC1A702692}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -57053,7 +57152,8 @@
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="21" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="21" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -57061,7 +57161,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="31" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="E1" s="31"/>
       <c r="F1" s="31"/>
@@ -57086,43 +57186,43 @@
         <v>94</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="38" t="s">
         <v>106</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -57134,13 +57234,13 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -57170,19 +57270,19 @@
         <v>15</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
@@ -57212,22 +57312,22 @@
         <v>15</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="6">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="E5" s="6">
         <v>16</v>
@@ -57255,18 +57355,18 @@
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="6">
         <v>1024</v>
@@ -57297,18 +57397,18 @@
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
@@ -57338,19 +57438,19 @@
         <v>9</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="6">
         <v>80</v>
@@ -57381,18 +57481,18 @@
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="6">
         <v>0</v>
@@ -57422,21 +57522,21 @@
         <v>9</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="6">
         <v>0</v>
@@ -57467,18 +57567,18 @@
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="6">
         <v>0</v>
@@ -57508,19 +57608,19 @@
         <v>9</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="6">
         <v>0</v>
@@ -57551,18 +57651,18 @@
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="6">
         <v>0</v>
@@ -57592,48 +57692,167 @@
         <v>15</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N13" s="6"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>126</v>
-      </c>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" s="35">
+        <v>8</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="G18" s="35">
+        <v>9</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="I18" s="35">
+        <v>10</v>
+      </c>
+      <c r="J18" s="35">
+        <v>6</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="L18" s="35">
+        <v>13</v>
+      </c>
+      <c r="M18" s="36">
+        <v>7</v>
+      </c>
+      <c r="N18" s="36"/>
+    </row>
+    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="N20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E25" s="6">
+        <v>16</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G25" s="6">
+        <v>16</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6">
+        <v>1792</v>
+      </c>
+      <c r="L25" s="6">
+        <v>9</v>
+      </c>
+      <c r="M25" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="N25" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="D1:N1"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -57644,7 +57863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADF9F42-C143-4CDD-8ACB-7652330B2E87}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -57653,22 +57872,22 @@
   <sheetData>
     <row r="1" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
@@ -57695,7 +57914,7 @@
         <v>$00</v>
       </c>
       <c r="H2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
@@ -57825,7 +58044,7 @@
         <v>$40</v>
       </c>
       <c r="H5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
@@ -58263,22 +58482,22 @@
     </row>
     <row r="28" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
@@ -58305,7 +58524,7 @@
         <v>$78</v>
       </c>
       <c r="H29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
@@ -58435,7 +58654,7 @@
         <v>$08</v>
       </c>
       <c r="H32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="3:31" x14ac:dyDescent="0.3">

</xml_diff>